<commit_message>
Work done till 15-06-2017 end
</commit_message>
<xml_diff>
--- a/api/MIS Reports/test2.xlsx
+++ b/api/MIS Reports/test2.xlsx
@@ -524,7 +524,7 @@
   <dimension ref="A1:AA2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -621,7 +621,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4">
-        <v>399475</v>
+        <v>435512</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
Work done till 17-06-2017
</commit_message>
<xml_diff>
--- a/api/MIS Reports/test2.xlsx
+++ b/api/MIS Reports/test2.xlsx
@@ -119,12 +119,6 @@
     <t>Maharashtra</t>
   </si>
   <si>
-    <t>Nath Valley School</t>
-  </si>
-  <si>
-    <t>Aurangabad</t>
-  </si>
-  <si>
     <t xml:space="preserve">P O Box 567, Cantonment Post Office, Satara Village, Paithan Road, </t>
   </si>
   <si>
@@ -147,6 +141,12 @@
   </si>
   <si>
     <t>Summer 2017</t>
+  </si>
+  <si>
+    <t>Sanskriti The Gurukul</t>
+  </si>
+  <si>
+    <t>Guwahati</t>
   </si>
 </sst>
 </file>
@@ -524,7 +524,7 @@
   <dimension ref="A1:AA2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -621,22 +621,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="4">
-        <v>435512</v>
+        <v>416793</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>34</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>29</v>
@@ -645,7 +645,7 @@
         <v>431002</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K2" s="4">
         <v>9960792266</v>
@@ -654,10 +654,10 @@
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
       <c r="O2" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="Q2" s="7">
         <v>43084</v>
@@ -678,13 +678,13 @@
         <v>28</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="X2" s="7">
         <v>43075</v>
       </c>
       <c r="Y2" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="Z2" s="4"/>
       <c r="AA2" s="4"/>

</xml_diff>